<commit_message>
add water mask By loginUser
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
+++ b/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225"/>
   </bookViews>
   <sheets>
     <sheet name="面部" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>Buy Plan</t>
   </si>
@@ -79,86 +79,6 @@
     <t>Part Name</t>
   </si>
   <si>
-    <t>&amp;=result.Factory</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.BuyPlanSeason</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.VersionNo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.DevSeason</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.DevTeam</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.Article</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.ModelNo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.ModelName</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.SampleNo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.DevStatus</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.DropDate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.ReleaseType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.CwaDeadline</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.ConfirmDate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.HpPartNo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.SupsName</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.TreatMent</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.PartName</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.ProcessDate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.CardDate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>底部色卡</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -175,14 +95,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&amp;=result.ProStatusId</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&amp;=result.Photo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Photo</t>
   </si>
   <si>
@@ -190,7 +102,136 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&amp;=result.Pdf</t>
+    <t>&amp;=result0.Factory</t>
+  </si>
+  <si>
+    <t>&amp;=result0.BuyPlanSeason</t>
+  </si>
+  <si>
+    <t>&amp;=result0.VersionNo</t>
+  </si>
+  <si>
+    <t>&amp;=result0.DevSeason</t>
+  </si>
+  <si>
+    <t>&amp;=result0.DevTeam</t>
+  </si>
+  <si>
+    <t>&amp;=result0.Article</t>
+  </si>
+  <si>
+    <t>&amp;=result0.CwaDeadline</t>
+  </si>
+  <si>
+    <t>&amp;=result0.ModelNo</t>
+  </si>
+  <si>
+    <t>&amp;=result0.DevStatus</t>
+  </si>
+  <si>
+    <t>&amp;=result0.DropDate</t>
+  </si>
+  <si>
+    <t>&amp;=result0.CardDate</t>
+  </si>
+  <si>
+    <t>&amp;=result0.ProcessDate</t>
+  </si>
+  <si>
+    <t>&amp;=result0.ReleaseType</t>
+  </si>
+  <si>
+    <t>&amp;=result0.SampleNo</t>
+  </si>
+  <si>
+    <t>&amp;=result0.ProStatusId</t>
+  </si>
+  <si>
+    <t>&amp;=result0.HpPartNo</t>
+  </si>
+  <si>
+    <t>&amp;=result0.SupsName</t>
+  </si>
+  <si>
+    <t>&amp;=result0.TreatMent</t>
+  </si>
+  <si>
+    <t>&amp;=result0.PartName</t>
+  </si>
+  <si>
+    <t>&amp;=result0.Photo</t>
+  </si>
+  <si>
+    <t>&amp;=result0.Pdf</t>
+  </si>
+  <si>
+    <t>&amp;=result1.Factory</t>
+  </si>
+  <si>
+    <t>&amp;=result1.BuyPlanSeason</t>
+  </si>
+  <si>
+    <t>&amp;=result1.VersionNo</t>
+  </si>
+  <si>
+    <t>&amp;=result1.DevSeason</t>
+  </si>
+  <si>
+    <t>&amp;=result1.DevTeam</t>
+  </si>
+  <si>
+    <t>&amp;=result1.Article</t>
+  </si>
+  <si>
+    <t>&amp;=result1.CwaDeadline</t>
+  </si>
+  <si>
+    <t>&amp;=result1.ModelNo</t>
+  </si>
+  <si>
+    <t>&amp;=result1.ModelName</t>
+  </si>
+  <si>
+    <t>&amp;=result1.DevStatus</t>
+  </si>
+  <si>
+    <t>&amp;=result1.DropDate</t>
+  </si>
+  <si>
+    <t>&amp;=result1.ConfirmDate</t>
+  </si>
+  <si>
+    <t>&amp;=result1.ProcessDate</t>
+  </si>
+  <si>
+    <t>&amp;=result1.ReleaseType</t>
+  </si>
+  <si>
+    <t>&amp;=result1.SampleNo</t>
+  </si>
+  <si>
+    <t>&amp;=result1.ProStatusId</t>
+  </si>
+  <si>
+    <t>&amp;=result1.HpPartNo</t>
+  </si>
+  <si>
+    <t>&amp;=result1.SupsName</t>
+  </si>
+  <si>
+    <t>&amp;=result1.TreatMent</t>
+  </si>
+  <si>
+    <t>&amp;=result1.PartName</t>
+  </si>
+  <si>
+    <t>&amp;=result1.Photo</t>
+  </si>
+  <si>
+    <t>&amp;=result1.Pdf</t>
+  </si>
+  <si>
+    <t>&amp;=result0.ModelName</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -632,11 +673,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4982"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1:V1"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -730,10 +771,10 @@
         <v>12</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>13</v>
@@ -742,7 +783,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>15</v>
@@ -757,78 +798,78 @@
         <v>18</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="V2" s="15" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="L3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="P3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>44</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="W3" s="13"/>
     </row>
@@ -30722,11 +30763,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+      <selection pane="bottomRight" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30816,10 +30857,10 @@
         <v>12</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>13</v>
@@ -30828,7 +30869,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>15</v>
@@ -30843,78 +30884,78 @@
         <v>18</v>
       </c>
       <c r="U2" s="15" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
f340 ppd excel export bug
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
+++ b/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
@@ -677,7 +677,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -701,8 +701,8 @@
     <col min="18" max="18" width="22.7109375" customWidth="1"/>
     <col min="19" max="19" width="18.85546875" customWidth="1"/>
     <col min="20" max="20" width="34.5703125" style="9" customWidth="1"/>
-    <col min="21" max="21" width="34.5703125" style="14" customWidth="1"/>
-    <col min="22" max="22" width="36.140625" customWidth="1"/>
+    <col min="21" max="21" width="34.5703125" style="14" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="36.140625" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -30764,10 +30764,10 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U5" sqref="U5"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30788,8 +30788,8 @@
     <col min="18" max="18" width="18.7109375" customWidth="1"/>
     <col min="19" max="19" width="17.7109375" customWidth="1"/>
     <col min="20" max="20" width="36.85546875" style="11" customWidth="1"/>
-    <col min="21" max="21" width="36.85546875" style="14" customWidth="1"/>
-    <col min="22" max="22" width="40.42578125" customWidth="1"/>
+    <col min="21" max="21" width="36.85546875" style="14" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="40.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
eng-authorize add only ui
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
+++ b/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="面部" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
   <si>
     <t>Buy Plan</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>&amp;=result0.ModelName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Photo Comment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result0.PhotoComment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result1.PhotoComment</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -239,7 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -264,13 +276,6 @@
       <name val="細明體"/>
       <family val="3"/>
       <charset val="136"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -308,9 +313,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -340,8 +344,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -357,9 +363,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -673,11 +678,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -700,10 +705,10 @@
     <col min="17" max="17" width="12.28515625" customWidth="1"/>
     <col min="18" max="18" width="22.7109375" customWidth="1"/>
     <col min="19" max="19" width="18.85546875" customWidth="1"/>
-    <col min="20" max="20" width="34.5703125" style="9" customWidth="1"/>
-    <col min="21" max="21" width="34.5703125" style="14" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="36.140625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" customWidth="1"/>
+    <col min="20" max="20" width="18" style="9" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" style="13" customWidth="1"/>
+    <col min="22" max="22" width="18" customWidth="1"/>
+    <col min="23" max="23" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" x14ac:dyDescent="0.2">
@@ -729,12 +734,13 @@
       </c>
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -800,8 +806,11 @@
       <c r="U2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="14" t="s">
         <v>24</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -871,13 +880,15 @@
       <c r="V3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="W3" s="13"/>
+      <c r="W3" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="N1:V1"/>
     <mergeCell ref="D1:M1"/>
+    <mergeCell ref="N1:W1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -887,13 +898,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -913,12 +924,13 @@
     <col min="17" max="17" width="15.7109375" customWidth="1"/>
     <col min="18" max="18" width="18.7109375" customWidth="1"/>
     <col min="19" max="19" width="17.7109375" customWidth="1"/>
-    <col min="20" max="20" width="36.85546875" style="11" customWidth="1"/>
-    <col min="21" max="21" width="36.85546875" style="14" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="40.42578125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="19.42578125" style="11" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" style="13" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" customWidth="1"/>
+    <col min="23" max="23" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -947,8 +959,9 @@
       <c r="T1" s="18"/>
       <c r="U1" s="18"/>
       <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
     </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1009,14 +1022,17 @@
       <c r="T2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="U2" s="14" t="s">
         <v>23</v>
       </c>
       <c r="V2" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="W2" s="15" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -1082,13 +1098,16 @@
       </c>
       <c r="V3" s="5" t="s">
         <v>67</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:M1"/>
-    <mergeCell ref="N1:V1"/>
+    <mergeCell ref="N1:W1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1.dtr-vs-list 1. f340ppd add fgt 3. try chart js
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
+++ b/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
   <si>
     <t>Buy Plan</t>
   </si>
@@ -244,6 +244,42 @@
   </si>
   <si>
     <t>&amp;=result1.PhotoComment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fgt FileName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fgt Remark</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result0.FgtReMark</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result0.FgtFileName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result1.FgtFileName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result1.FgtReMark</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result1.FgtHyperLink</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fgt Result</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result0.FgtHyperLink</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -316,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -351,17 +387,27 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -676,13 +722,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V11" sqref="V11"/>
+      <selection pane="bottomRight" activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -709,40 +755,46 @@
     <col min="21" max="21" width="15.28515625" style="13" customWidth="1"/>
     <col min="22" max="22" width="18" customWidth="1"/>
     <col min="23" max="23" width="30.42578125" customWidth="1"/>
+    <col min="24" max="24" width="19.7109375" style="16" customWidth="1"/>
+    <col min="25" max="25" width="22.5703125" style="16" customWidth="1"/>
+    <col min="26" max="26" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="18" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="22"/>
     </row>
-    <row r="2" spans="1:23" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -812,8 +864,17 @@
       <c r="W2" s="15" t="s">
         <v>69</v>
       </c>
+      <c r="X2" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -882,13 +943,22 @@
       </c>
       <c r="W3" s="5" t="s">
         <v>70</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:M1"/>
-    <mergeCell ref="N1:W1"/>
+    <mergeCell ref="N1:Z1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -898,13 +968,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
+      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -928,40 +998,46 @@
     <col min="21" max="21" width="19.42578125" style="13" customWidth="1"/>
     <col min="22" max="22" width="19.42578125" customWidth="1"/>
     <col min="23" max="23" width="27" customWidth="1"/>
+    <col min="24" max="24" width="16.5703125" customWidth="1"/>
+    <col min="25" max="25" width="23.140625" customWidth="1"/>
+    <col min="26" max="26" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="18" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="22"/>
     </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1031,8 +1107,17 @@
       <c r="W2" s="15" t="s">
         <v>69</v>
       </c>
+      <c r="X2" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -1101,15 +1186,25 @@
       </c>
       <c r="W3" s="5" t="s">
         <v>71</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:M1"/>
-    <mergeCell ref="N1:W1"/>
+    <mergeCell ref="N1:Z1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
F340-ppd color code fix
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
+++ b/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
@@ -15,12 +15,16 @@
     <sheet name="面部" sheetId="1" r:id="rId1"/>
     <sheet name="底部" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">底部!$A$2:$Y$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">面部!$A$2:$Y$2</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>Buy Plan</t>
   </si>
@@ -275,11 +279,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Fgt Result</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>&amp;=result0.FgtHyperLink</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>QC Team</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fgt FileName</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -287,7 +295,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -313,8 +321,22 @@
       <family val="3"/>
       <charset val="136"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,6 +361,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -352,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -388,24 +416,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -414,6 +443,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFD966"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -722,13 +756,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AZ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z3" sqref="Z3"/>
+      <selection pane="bottomRight" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -760,16 +794,16 @@
     <col min="26" max="26" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="20"/>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
@@ -778,23 +812,25 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="22"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="17"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -865,16 +901,13 @@
         <v>69</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y2" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z2" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y2" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -945,20 +978,22 @@
         <v>70</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z3" s="5" t="s">
         <v>74</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <autoFilter ref="A2:Y2"/>
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:M1"/>
-    <mergeCell ref="N1:Z1"/>
+    <mergeCell ref="N1:W1"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -968,13 +1003,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AY3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -998,46 +1033,46 @@
     <col min="21" max="21" width="19.42578125" style="13" customWidth="1"/>
     <col min="22" max="22" width="19.42578125" customWidth="1"/>
     <col min="23" max="23" width="27" customWidth="1"/>
-    <col min="24" max="24" width="16.5703125" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" customWidth="1"/>
-    <col min="26" max="26" width="26.85546875" customWidth="1"/>
+    <col min="24" max="24" width="23.140625" customWidth="1"/>
+    <col min="25" max="25" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:51" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="23" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y1" s="23"/>
     </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:51" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1108,16 +1143,13 @@
         <v>69</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y2" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="Y2" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:51" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -1188,20 +1220,22 @@
         <v>71</v>
       </c>
       <c r="X3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY3" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <autoFilter ref="A2:Y2"/>
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:M1"/>
-    <mergeCell ref="N1:Z1"/>
+    <mergeCell ref="N1:W1"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
F340 ppd bug fix
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
+++ b/DKS-API/Resources/Template/TempF340PPDProcessTabs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225"/>
   </bookViews>
   <sheets>
     <sheet name="面部" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
   <si>
     <t>Buy Plan</t>
   </si>
@@ -83,18 +83,6 @@
     <t>Part Name</t>
   </si>
   <si>
-    <t>底部色卡</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">跨單位作業流程 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>面部實物卡</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ProStatusId</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -136,9 +124,6 @@
     <t>&amp;=result0.DropDate</t>
   </si>
   <si>
-    <t>&amp;=result0.CardDate</t>
-  </si>
-  <si>
     <t>&amp;=result0.ProcessDate</t>
   </si>
   <si>
@@ -202,9 +187,6 @@
     <t>&amp;=result1.DropDate</t>
   </si>
   <si>
-    <t>&amp;=result1.ConfirmDate</t>
-  </si>
-  <si>
     <t>&amp;=result1.ProcessDate</t>
   </si>
   <si>
@@ -288,6 +270,34 @@
   </si>
   <si>
     <t>Fgt FileName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result0.ConfirmDate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result1.CardDate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部色卡日期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>跨單位作業流程日期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>部品圖片</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PDF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>面部實物卡日期</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -380,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -423,19 +433,22 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,31 +771,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W2" sqref="W2"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="34.28515625" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
-    <col min="12" max="13" width="19.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" customWidth="1"/>
     <col min="15" max="15" width="20.42578125" customWidth="1"/>
     <col min="16" max="16" width="26.140625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
     <col min="18" max="18" width="22.7109375" customWidth="1"/>
     <col min="19" max="19" width="18.85546875" customWidth="1"/>
     <col min="20" max="20" width="18" style="9" customWidth="1"/>
@@ -798,12 +812,12 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
@@ -812,22 +826,22 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y1" s="23"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" s="25"/>
       <c r="Z1" s="17"/>
     </row>
     <row r="2" spans="1:52" ht="16.5" x14ac:dyDescent="0.2">
@@ -865,10 +879,10 @@
         <v>12</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>13</v>
@@ -877,7 +891,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>15</v>
@@ -892,99 +906,99 @@
         <v>18</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W2" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="Y2" s="18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:52" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="I3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="L3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="W3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="X3" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="Y3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="AZ3" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1005,16 +1019,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
@@ -1022,7 +1037,7 @@
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" customWidth="1"/>
     <col min="12" max="12" width="21.140625" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" customWidth="1"/>
     <col min="14" max="14" width="19.42578125" customWidth="1"/>
     <col min="15" max="15" width="26.140625" customWidth="1"/>
     <col min="16" max="16" width="26.140625" style="7" customWidth="1"/>
@@ -1043,19 +1058,19 @@
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="21" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="22"/>
@@ -1067,10 +1082,10 @@
       <c r="U1" s="22"/>
       <c r="V1" s="22"/>
       <c r="W1" s="22"/>
-      <c r="X1" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y1" s="23"/>
+      <c r="X1" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" s="25"/>
     </row>
     <row r="2" spans="1:51" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1107,10 +1122,10 @@
         <v>12</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>13</v>
@@ -1119,7 +1134,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>15</v>
@@ -1133,100 +1148,100 @@
       <c r="T2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="14" t="s">
-        <v>23</v>
+      <c r="U2" s="26" t="s">
+        <v>81</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="W2" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Y2" s="18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:51" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="L3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="U3" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="V3" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="W3" s="5" t="s">
+      <c r="X3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="X3" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="Y3" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AY3" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>